<commit_message>
Protoparvovirus EPV component added
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/AAV-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485A3CFA-16F6-4841-8569-B9DDD65D51FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513CB1CC-02E6-E24C-A102-A12EA320778F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3799,7 +3799,7 @@
   <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="A1:W57"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding avian and reptile dependos
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513CB1CC-02E6-E24C-A102-A12EA320778F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3979B9E-11A4-6343-A2BB-79859C9BB1D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13400" yWindow="540" windowWidth="32040" windowHeight="20020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -20,8 +20,16 @@
     <sheet name="Sheet3" sheetId="7" r:id="rId5"/>
     <sheet name="bats" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="413">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -1031,12 +1039,6 @@
     <t>epv-dependo.62-sarcophilus</t>
   </si>
   <si>
-    <t>epv-dependo.65-passeriformes</t>
-  </si>
-  <si>
-    <t>epv-dependo.66-passeriformes</t>
-  </si>
-  <si>
     <t>dependo.35-rhinolophidae-con</t>
   </si>
   <si>
@@ -1227,6 +1229,54 @@
   </si>
   <si>
     <t>ncbi-refseqs-dependo-epv</t>
+  </si>
+  <si>
+    <t>dependo.165-passeriformes-con</t>
+  </si>
+  <si>
+    <t>dependo.166-passeriformes-con</t>
+  </si>
+  <si>
+    <t>dependo.165-passeriformes</t>
+  </si>
+  <si>
+    <t>epv-dependo.165-passeriformes</t>
+  </si>
+  <si>
+    <t>epv-dependo.166-passeriformes</t>
+  </si>
+  <si>
+    <t>Pelecanus</t>
+  </si>
+  <si>
+    <t>Thamnophis</t>
+  </si>
+  <si>
+    <t>Gekko</t>
+  </si>
+  <si>
+    <t>dependo.202-gekko</t>
+  </si>
+  <si>
+    <t>dependo.201.1-thamnophis</t>
+  </si>
+  <si>
+    <t>dependo.201.2-thamnophis</t>
+  </si>
+  <si>
+    <t>PCGF5</t>
+  </si>
+  <si>
+    <t>ANKRD1</t>
+  </si>
+  <si>
+    <t>AFF1</t>
+  </si>
+  <si>
+    <t>PTPN13</t>
+  </si>
+  <si>
+    <t>dependo.170-pelecanus</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1443,6 +1493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2394,7 +2450,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2511,6 +2567,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="939">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3798,8 +3855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="A1:W61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3833,7 +3890,7 @@
         <v>209</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -3842,10 +3899,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>261</v>
@@ -3904,7 +3961,7 @@
         <v>87</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D2" s="59" t="s">
         <v>2</v>
@@ -3913,19 +3970,19 @@
         <v>3</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G2" s="61" t="s">
         <v>137</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I2" s="61" t="s">
         <v>137</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K2" s="61" t="s">
         <v>137</v>
@@ -3973,7 +4030,7 @@
         <v>78</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D3" s="59" t="s">
         <v>2</v>
@@ -3982,19 +4039,19 @@
         <v>3</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>246</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>246</v>
@@ -4023,7 +4080,9 @@
       <c r="S3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="11"/>
+      <c r="T3" s="11">
+        <v>32913662</v>
+      </c>
       <c r="U3" s="11" t="s">
         <v>7</v>
       </c>
@@ -4042,7 +4101,7 @@
         <v>85</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D4" s="59" t="s">
         <v>2</v>
@@ -4051,22 +4110,22 @@
         <v>3</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G4" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I4" s="49" t="s">
         <v>280</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K4" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>244</v>
@@ -4090,7 +4149,9 @@
       <c r="S4" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="T4" s="11"/>
+      <c r="T4" s="11">
+        <v>32913662</v>
+      </c>
       <c r="U4" s="12" t="s">
         <v>109</v>
       </c>
@@ -4109,7 +4170,7 @@
         <v>86</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D5" s="59" t="s">
         <v>2</v>
@@ -4118,22 +4179,22 @@
         <v>3</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G5" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I5" s="49" t="s">
         <v>280</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K5" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>244</v>
@@ -4159,7 +4220,9 @@
       <c r="S5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="T5" s="11"/>
+      <c r="T5" s="11">
+        <v>32913662</v>
+      </c>
       <c r="U5" s="11" t="s">
         <v>10</v>
       </c>
@@ -4178,7 +4241,7 @@
         <v>95</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D6" s="59" t="s">
         <v>2</v>
@@ -4187,19 +4250,19 @@
         <v>3</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>246</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>246</v>
@@ -4247,7 +4310,7 @@
         <v>193</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>2</v>
@@ -4256,10 +4319,10 @@
         <v>3</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G7" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H7" s="44" t="s">
         <v>94</v>
@@ -4268,10 +4331,10 @@
         <v>94</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K7" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>244</v>
@@ -4316,7 +4379,7 @@
         <v>235</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D8" s="59" t="s">
         <v>2</v>
@@ -4325,16 +4388,16 @@
         <v>3</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G8" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H8" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I8" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J8" s="44" t="s">
         <v>94</v>
@@ -4383,7 +4446,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D9" s="59" t="s">
         <v>2</v>
@@ -4392,16 +4455,16 @@
         <v>3</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G9" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I9" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J9" s="44" t="s">
         <v>94</v>
@@ -4450,7 +4513,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D10" s="59" t="s">
         <v>2</v>
@@ -4459,10 +4522,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G10" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H10" s="44" t="s">
         <v>94</v>
@@ -4471,10 +4534,10 @@
         <v>94</v>
       </c>
       <c r="J10" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K10" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>244</v>
@@ -4517,7 +4580,7 @@
         <v>236</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D11" s="59" t="s">
         <v>2</v>
@@ -4526,16 +4589,16 @@
         <v>3</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G11" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I11" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J11" s="44" t="s">
         <v>94</v>
@@ -4570,7 +4633,7 @@
         <v>236</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="W11" s="30" t="s">
         <v>3</v>
@@ -4584,7 +4647,7 @@
         <v>107</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D12" s="59" t="s">
         <v>2</v>
@@ -4593,16 +4656,16 @@
         <v>3</v>
       </c>
       <c r="F12" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G12" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J12" s="44" t="s">
         <v>94</v>
@@ -4651,7 +4714,7 @@
         <v>104</v>
       </c>
       <c r="C13" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D13" s="59" t="s">
         <v>2</v>
@@ -4660,16 +4723,16 @@
         <v>3</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G13" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I13" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J13" s="44" t="s">
         <v>94</v>
@@ -4718,7 +4781,7 @@
         <v>192</v>
       </c>
       <c r="C14" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D14" s="59" t="s">
         <v>2</v>
@@ -4727,22 +4790,22 @@
         <v>3</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G14" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H14" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I14" s="49" t="s">
         <v>280</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K14" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>244</v>
@@ -4785,7 +4848,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D15" s="59" t="s">
         <v>2</v>
@@ -4794,22 +4857,22 @@
         <v>3</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H15" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I15" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J15" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K15" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L15" s="50" t="s">
         <v>282</v>
@@ -4854,7 +4917,7 @@
         <v>113</v>
       </c>
       <c r="C16" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D16" s="59" t="s">
         <v>2</v>
@@ -4863,16 +4926,16 @@
         <v>3</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H16" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I16" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J16" s="44" t="s">
         <v>94</v>
@@ -4923,7 +4986,7 @@
         <v>237</v>
       </c>
       <c r="C17" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D17" s="59" t="s">
         <v>2</v>
@@ -4932,16 +4995,16 @@
         <v>3</v>
       </c>
       <c r="F17" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I17" s="43" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J17" s="44" t="s">
         <v>94</v>
@@ -4992,7 +5055,7 @@
         <v>214</v>
       </c>
       <c r="C18" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D18" s="59" t="s">
         <v>2</v>
@@ -5001,7 +5064,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>246</v>
@@ -5013,7 +5076,7 @@
         <v>94</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>246</v>
@@ -5059,7 +5122,7 @@
         <v>240</v>
       </c>
       <c r="C19" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D19" s="59" t="s">
         <v>2</v>
@@ -5068,16 +5131,16 @@
         <v>3</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G19" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I19" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J19" s="44" t="s">
         <v>94</v>
@@ -5109,7 +5172,7 @@
       </c>
       <c r="T19" s="12"/>
       <c r="U19" s="11" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="V19" s="11" t="s">
         <v>312</v>
@@ -5126,7 +5189,7 @@
         <v>238</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D20" s="59" t="s">
         <v>2</v>
@@ -5135,16 +5198,16 @@
         <v>3</v>
       </c>
       <c r="F20" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G20" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I20" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J20" s="44" t="s">
         <v>94</v>
@@ -5195,7 +5258,7 @@
         <v>101</v>
       </c>
       <c r="C21" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D21" s="59" t="s">
         <v>2</v>
@@ -5204,7 +5267,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>246</v>
@@ -5216,7 +5279,7 @@
         <v>94</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>246</v>
@@ -5266,7 +5329,7 @@
         <v>89</v>
       </c>
       <c r="C22" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D22" s="59" t="s">
         <v>2</v>
@@ -5275,7 +5338,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>246</v>
@@ -5287,7 +5350,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>246</v>
@@ -5337,7 +5400,7 @@
         <v>176</v>
       </c>
       <c r="C23" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D23" s="59" t="s">
         <v>2</v>
@@ -5346,16 +5409,16 @@
         <v>3</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G23" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H23" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I23" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J23" s="44" t="s">
         <v>94</v>
@@ -5404,7 +5467,7 @@
         <v>216</v>
       </c>
       <c r="C24" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D24" s="59" t="s">
         <v>2</v>
@@ -5413,19 +5476,19 @@
         <v>3</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>246</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>246</v>
@@ -5468,10 +5531,10 @@
         <v>30</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C25" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D25" s="59" t="s">
         <v>2</v>
@@ -5480,19 +5543,19 @@
         <v>3</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>246</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>246</v>
@@ -5521,10 +5584,10 @@
       </c>
       <c r="T25" s="11"/>
       <c r="U25" s="48" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V25" s="48" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="W25" s="13" t="s">
         <v>3</v>
@@ -5535,10 +5598,10 @@
         <v>31</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C26" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D26" s="59" t="s">
         <v>2</v>
@@ -5559,7 +5622,7 @@
         <v>145</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>246</v>
@@ -5588,10 +5651,10 @@
       </c>
       <c r="T26" s="11"/>
       <c r="U26" s="48" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="V26" s="48" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="W26" s="13" t="s">
         <v>3</v>
@@ -5602,10 +5665,10 @@
         <v>32</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D27" s="59" t="s">
         <v>2</v>
@@ -5614,19 +5677,19 @@
         <v>3</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>246</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>246</v>
@@ -5655,10 +5718,10 @@
       </c>
       <c r="T27" s="11"/>
       <c r="U27" s="48" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="V27" s="48" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="W27" s="13" t="s">
         <v>3</v>
@@ -5669,10 +5732,10 @@
         <v>33</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C28" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D28" s="59" t="s">
         <v>2</v>
@@ -5681,13 +5744,13 @@
         <v>3</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>246</v>
@@ -5722,10 +5785,10 @@
       </c>
       <c r="T28" s="11"/>
       <c r="U28" s="48" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="V28" s="48" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="W28" s="13" t="s">
         <v>3</v>
@@ -5736,10 +5799,10 @@
         <v>34</v>
       </c>
       <c r="B29" s="59" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C29" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D29" s="59" t="s">
         <v>2</v>
@@ -5785,14 +5848,14 @@
         <v>242</v>
       </c>
       <c r="S29" s="48" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="T29" s="11"/>
       <c r="U29" s="48" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="V29" s="48" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="W29" s="13" t="s">
         <v>3</v>
@@ -5803,10 +5866,10 @@
         <v>35</v>
       </c>
       <c r="B30" s="59" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C30" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D30" s="59" t="s">
         <v>2</v>
@@ -5815,22 +5878,22 @@
         <v>3</v>
       </c>
       <c r="F30" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G30" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H30" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I30" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J30" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K30" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L30" s="48" t="s">
         <v>244</v>
@@ -5852,14 +5915,14 @@
         <v>75</v>
       </c>
       <c r="S30" s="11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="T30" s="11"/>
       <c r="U30" s="48" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="V30" s="48" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="W30" s="13" t="s">
         <v>3</v>
@@ -5870,10 +5933,10 @@
         <v>36</v>
       </c>
       <c r="B31" s="59" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C31" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D31" s="59" t="s">
         <v>2</v>
@@ -5882,16 +5945,16 @@
         <v>3</v>
       </c>
       <c r="F31" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G31" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H31" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I31" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J31" s="44" t="s">
         <v>94</v>
@@ -5919,14 +5982,14 @@
         <v>75</v>
       </c>
       <c r="S31" s="11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="T31" s="11"/>
       <c r="U31" s="48" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="V31" s="48" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="W31" s="13" t="s">
         <v>3</v>
@@ -5937,10 +6000,10 @@
         <v>39</v>
       </c>
       <c r="B32" s="59" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C32" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D32" s="59" t="s">
         <v>2</v>
@@ -5949,13 +6012,13 @@
         <v>3</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>246</v>
@@ -5993,7 +6056,7 @@
         <v>287</v>
       </c>
       <c r="V32" s="11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="W32" s="13" t="s">
         <v>3</v>
@@ -6004,10 +6067,10 @@
         <v>39</v>
       </c>
       <c r="B33" s="59" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C33" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D33" s="59" t="s">
         <v>2</v>
@@ -6016,13 +6079,13 @@
         <v>3</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I33" s="6" t="s">
         <v>246</v>
@@ -6057,7 +6120,7 @@
       </c>
       <c r="T33" s="11"/>
       <c r="U33" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="V33" s="11" t="s">
         <v>323</v>
@@ -6071,10 +6134,10 @@
         <v>40</v>
       </c>
       <c r="B34" s="59" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C34" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D34" s="59" t="s">
         <v>2</v>
@@ -6083,13 +6146,13 @@
         <v>3</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>246</v>
@@ -6138,10 +6201,10 @@
         <v>42</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C35" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D35" s="59" t="s">
         <v>2</v>
@@ -6150,16 +6213,16 @@
         <v>3</v>
       </c>
       <c r="F35" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G35" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H35" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I35" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J35" s="44" t="s">
         <v>94</v>
@@ -6187,14 +6250,14 @@
         <v>74</v>
       </c>
       <c r="S35" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="T35" s="11"/>
       <c r="U35" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="V35" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="W35" s="30" t="s">
         <v>3</v>
@@ -6205,10 +6268,10 @@
         <v>43</v>
       </c>
       <c r="B36" s="59" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C36" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D36" s="59" t="s">
         <v>2</v>
@@ -6217,13 +6280,13 @@
         <v>3</v>
       </c>
       <c r="F36" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G36" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H36" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I36" s="49" t="s">
         <v>280</v>
@@ -6258,10 +6321,10 @@
       </c>
       <c r="T36" s="12"/>
       <c r="U36" s="59" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="V36" s="59" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="W36" s="30" t="s">
         <v>3</v>
@@ -6275,7 +6338,7 @@
         <v>105</v>
       </c>
       <c r="C37" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D37" s="59" t="s">
         <v>2</v>
@@ -6341,10 +6404,10 @@
         <v>45</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C38" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D38" s="59" t="s">
         <v>2</v>
@@ -6353,13 +6416,13 @@
         <v>3</v>
       </c>
       <c r="F38" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G38" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H38" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I38" s="49" t="s">
         <v>280</v>
@@ -6394,10 +6457,10 @@
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="V38" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="W38" s="30" t="s">
         <v>3</v>
@@ -6411,7 +6474,7 @@
         <v>274</v>
       </c>
       <c r="C39" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D39" s="59" t="s">
         <v>2</v>
@@ -6420,22 +6483,22 @@
         <v>3</v>
       </c>
       <c r="F39" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G39" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H39" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I39" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J39" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K39" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L39" s="46" t="s">
         <v>244</v>
@@ -6478,7 +6541,7 @@
         <v>200</v>
       </c>
       <c r="C40" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D40" s="59" t="s">
         <v>2</v>
@@ -6487,16 +6550,16 @@
         <v>3</v>
       </c>
       <c r="F40" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G40" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I40" s="60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>145</v>
@@ -6528,10 +6591,10 @@
       </c>
       <c r="T40" s="11"/>
       <c r="U40" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="V40" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="W40" s="30" t="s">
         <v>3</v>
@@ -6542,10 +6605,10 @@
         <v>50</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D41" s="59" t="s">
         <v>2</v>
@@ -6594,10 +6657,10 @@
         <v>70</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="V41" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="W41" s="13" t="s">
         <v>3</v>
@@ -6608,10 +6671,10 @@
         <v>51</v>
       </c>
       <c r="B42" s="59" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C42" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D42" s="59" t="s">
         <v>2</v>
@@ -6661,10 +6724,10 @@
       </c>
       <c r="T42" s="11"/>
       <c r="U42" s="11" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="V42" s="11" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="W42" s="30" t="s">
         <v>3</v>
@@ -6675,10 +6738,10 @@
         <v>53</v>
       </c>
       <c r="B43" s="59" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C43" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D43" s="59" t="s">
         <v>2</v>
@@ -6687,13 +6750,13 @@
         <v>3</v>
       </c>
       <c r="F43" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G43" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I43" s="49" t="s">
         <v>280</v>
@@ -6728,10 +6791,10 @@
       </c>
       <c r="T43" s="11"/>
       <c r="U43" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="V43" s="11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="W43" s="13" t="s">
         <v>3</v>
@@ -6742,10 +6805,10 @@
         <v>54</v>
       </c>
       <c r="B44" s="59" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C44" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D44" s="59" t="s">
         <v>2</v>
@@ -6754,13 +6817,13 @@
         <v>3</v>
       </c>
       <c r="F44" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G44" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I44" s="49" t="s">
         <v>280</v>
@@ -6795,10 +6858,10 @@
       </c>
       <c r="T44" s="11"/>
       <c r="U44" s="59" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="V44" s="59" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="W44" s="13" t="s">
         <v>3</v>
@@ -6812,7 +6875,7 @@
         <v>267</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D45" s="59" t="s">
         <v>2</v>
@@ -6865,7 +6928,7 @@
         <v>267</v>
       </c>
       <c r="V45" s="46" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="W45" s="13" t="s">
         <v>3</v>
@@ -6876,10 +6939,10 @@
         <v>56</v>
       </c>
       <c r="B46" s="59" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D46" s="59" t="s">
         <v>2</v>
@@ -6888,13 +6951,13 @@
         <v>3</v>
       </c>
       <c r="F46" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G46" s="49" t="s">
         <v>280</v>
       </c>
       <c r="H46" s="43" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I46" s="49" t="s">
         <v>280</v>
@@ -6928,10 +6991,10 @@
       </c>
       <c r="T46" s="11"/>
       <c r="U46" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="W46" s="13" t="s">
         <v>3</v>
@@ -6945,7 +7008,7 @@
         <v>222</v>
       </c>
       <c r="C47" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D47" s="59" t="s">
         <v>2</v>
@@ -6954,13 +7017,13 @@
         <v>3</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>246</v>
@@ -7012,7 +7075,7 @@
         <v>221</v>
       </c>
       <c r="C48" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D48" s="59" t="s">
         <v>2</v>
@@ -7021,16 +7084,16 @@
         <v>3</v>
       </c>
       <c r="F48" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G48" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H48" s="57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I48" s="57" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J48" s="44" t="s">
         <v>94</v>
@@ -7078,7 +7141,7 @@
         <v>103</v>
       </c>
       <c r="C49" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D49" s="59" t="s">
         <v>2</v>
@@ -7087,13 +7150,13 @@
         <v>3</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>246</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>246</v>
@@ -7145,7 +7208,7 @@
         <v>157</v>
       </c>
       <c r="C50" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D50" s="59" t="s">
         <v>2</v>
@@ -7212,7 +7275,7 @@
         <v>158</v>
       </c>
       <c r="C51" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D51" s="59" t="s">
         <v>2</v>
@@ -7279,7 +7342,7 @@
         <v>159</v>
       </c>
       <c r="C52" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D52" s="59" t="s">
         <v>2</v>
@@ -7340,13 +7403,13 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" s="59">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>79</v>
+        <v>397</v>
       </c>
       <c r="C53" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D53" s="59" t="s">
         <v>2</v>
@@ -7378,11 +7441,11 @@
       <c r="M53" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="N53" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="O53" s="36" t="s">
-        <v>145</v>
+      <c r="N53" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="O53" s="35" t="s">
+        <v>408</v>
       </c>
       <c r="P53" s="32" t="s">
         <v>145</v>
@@ -7396,10 +7459,10 @@
       </c>
       <c r="T53" s="31"/>
       <c r="U53" s="33" t="s">
-        <v>13</v>
+        <v>399</v>
       </c>
       <c r="V53" s="33" t="s">
-        <v>333</v>
+        <v>400</v>
       </c>
       <c r="W53" s="34" t="s">
         <v>3</v>
@@ -7407,13 +7470,13 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" s="59">
-        <v>66</v>
+        <v>166</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>80</v>
+        <v>398</v>
       </c>
       <c r="C54" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D54" s="59" t="s">
         <v>2</v>
@@ -7445,11 +7508,11 @@
       <c r="M54" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="N54" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="O54" s="36" t="s">
-        <v>145</v>
+      <c r="N54" s="35" t="s">
+        <v>411</v>
+      </c>
+      <c r="O54" s="35" t="s">
+        <v>410</v>
       </c>
       <c r="P54" s="32" t="s">
         <v>145</v>
@@ -7463,10 +7526,10 @@
       </c>
       <c r="T54" s="31"/>
       <c r="U54" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="V54" s="33" t="s">
-        <v>334</v>
+        <v>401</v>
+      </c>
+      <c r="V54" s="62" t="s">
+        <v>401</v>
       </c>
       <c r="W54" s="34" t="s">
         <v>3</v>
@@ -7477,10 +7540,10 @@
         <v>500</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C55" s="59" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D55" s="59" t="s">
         <v>2</v>
@@ -7489,16 +7552,16 @@
         <v>3</v>
       </c>
       <c r="F55" s="43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G55" s="43" t="s">
+        <v>378</v>
+      </c>
+      <c r="H55" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="H55" s="43" t="s">
-        <v>382</v>
-      </c>
       <c r="I55" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J55" s="44" t="s">
         <v>94</v>
@@ -7526,14 +7589,14 @@
         <v>74</v>
       </c>
       <c r="S55" s="58" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="T55" s="11"/>
       <c r="U55" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V55" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="W55" s="13" t="s">
         <v>3</v>
@@ -7544,10 +7607,10 @@
         <v>500</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C56" s="59" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D56" s="59" t="s">
         <v>2</v>
@@ -7556,16 +7619,16 @@
         <v>3</v>
       </c>
       <c r="F56" s="43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G56" s="43" t="s">
+        <v>378</v>
+      </c>
+      <c r="H56" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="H56" s="43" t="s">
-        <v>382</v>
-      </c>
       <c r="I56" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J56" s="44" t="s">
         <v>94</v>
@@ -7593,14 +7656,14 @@
         <v>74</v>
       </c>
       <c r="S56" s="58" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="T56" s="11"/>
       <c r="U56" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="V56" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="W56" s="30" t="s">
         <v>3</v>
@@ -7610,11 +7673,11 @@
       <c r="A57" s="59">
         <v>500</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="C57" s="59" t="s">
         <v>395</v>
-      </c>
-      <c r="C57" s="59" t="s">
-        <v>397</v>
       </c>
       <c r="D57" s="59" t="s">
         <v>2</v>
@@ -7623,16 +7686,16 @@
         <v>3</v>
       </c>
       <c r="F57" s="43" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G57" s="43" t="s">
+        <v>378</v>
+      </c>
+      <c r="H57" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="H57" s="43" t="s">
-        <v>382</v>
-      </c>
       <c r="I57" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J57" s="44" t="s">
         <v>94</v>
@@ -7660,29 +7723,281 @@
         <v>74</v>
       </c>
       <c r="S57" s="58" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="U57" t="s">
+        <v>393</v>
+      </c>
+      <c r="V57" t="s">
+        <v>394</v>
+      </c>
+      <c r="W57" s="30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A58" s="59">
+        <v>202</v>
+      </c>
+      <c r="B58" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="C58" s="59" t="s">
         <v>395</v>
       </c>
-      <c r="V57" t="s">
-        <v>396</v>
-      </c>
-      <c r="W57" s="30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58"/>
+      <c r="D58" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J58" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K58" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L58" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="M58" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="N58" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="O58" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="P58" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S58" s="58" t="s">
+        <v>404</v>
+      </c>
+      <c r="U58" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="V58" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="W58" s="34" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A59"/>
+      <c r="A59" s="59">
+        <v>201.1</v>
+      </c>
+      <c r="B59" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="C59" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="D59" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J59" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K59" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L59" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="M59" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="N59" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="O59" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="P59" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S59" s="58" t="s">
+        <v>403</v>
+      </c>
+      <c r="U59" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="V59" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="W59" s="13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A60"/>
+      <c r="A60" s="59">
+        <v>201.2</v>
+      </c>
+      <c r="B60" s="59" t="s">
+        <v>407</v>
+      </c>
+      <c r="C60" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="D60" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J60" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K60" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L60" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="M60" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="N60" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="O60" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="P60" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S60" s="58" t="s">
+        <v>403</v>
+      </c>
+      <c r="U60" s="59" t="s">
+        <v>407</v>
+      </c>
+      <c r="V60" s="59" t="s">
+        <v>407</v>
+      </c>
+      <c r="W60" s="30" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A61"/>
+      <c r="A61" s="59">
+        <v>170</v>
+      </c>
+      <c r="B61" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C61" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="D61" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J61" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K61" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L61" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="M61" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="N61" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="O61" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="P61" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S61" s="58" t="s">
+        <v>402</v>
+      </c>
+      <c r="U61" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="V61" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="W61" s="30" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62"/>
@@ -7736,7 +8051,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>244</v>
@@ -7777,10 +8092,10 @@
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="48" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="R3" s="48" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="S3" s="13" t="s">
         <v>3</v>
@@ -10188,7 +10503,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B35" s="29">
         <v>48</v>
@@ -11194,7 +11509,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C4" s="48" t="s">
         <v>244</v>
@@ -11308,7 +11623,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C6" s="48" t="s">
         <v>244</v>
@@ -11366,7 +11681,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C7" s="48" t="s">
         <v>244</v>

</xml_diff>

<commit_message>
Incorporated more dependo EPVs. Rebuilt dependo genus phylogenyies with new EPVs included.
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6C473-FB30-1541-B030-27E60C2A3EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779CB772-600F-2D4E-AAC6-75BF52BAAC67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11680" yWindow="3160" windowWidth="37760" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3883,7 +3883,7 @@
   <dimension ref="A1:Y72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="D15" sqref="A1:W66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Incorporated marsupial and reptile EPV dependos
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50D229B-3ECB-7346-91A9-EC31A9A024B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CA9F68-6890-A449-8F94-16B610A179A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="13380" windowWidth="37760" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6560" yWindow="3700" windowWidth="37760" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2114" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2114" uniqueCount="433">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -1229,12 +1229,6 @@
   </si>
   <si>
     <t>ncbi-refseqs-dependo-epv</t>
-  </si>
-  <si>
-    <t>dependo.165-passeriformes-con</t>
-  </si>
-  <si>
-    <t>dependo.166-passeriformes-con</t>
   </si>
   <si>
     <t>dependo.165-passeriformes</t>
@@ -3921,8 +3915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4209,7 +4203,7 @@
         <v>32913662</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="V4" s="12" t="s">
         <v>298</v>
@@ -7315,7 +7309,7 @@
         <v>63</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C53" s="59" t="s">
         <v>395</v>
@@ -7363,13 +7357,13 @@
         <v>58</v>
       </c>
       <c r="S53" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="V53" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="W53" s="12"/>
       <c r="X53" s="12"/>
@@ -7379,7 +7373,7 @@
         <v>80</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C54" s="59" t="s">
         <v>395</v>
@@ -7428,13 +7422,13 @@
         <v>58</v>
       </c>
       <c r="S54" s="59" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="U54" s="59" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="V54" s="59" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="W54" s="12"/>
       <c r="X54" s="12"/>
@@ -7444,7 +7438,7 @@
         <v>81</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C55" s="59" t="s">
         <v>395</v>
@@ -7493,13 +7487,13 @@
         <v>58</v>
       </c>
       <c r="S55" s="59" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="U55" s="59" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="V55" s="59" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="W55" s="12"/>
       <c r="X55" s="12"/>
@@ -7509,7 +7503,7 @@
         <v>82</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C56" s="59" t="s">
         <v>395</v>
@@ -7558,13 +7552,13 @@
         <v>58</v>
       </c>
       <c r="S56" s="59" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="U56" s="59" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="V56" s="59" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="W56" s="12"/>
       <c r="X56" s="12"/>
@@ -7610,10 +7604,10 @@
         <v>285</v>
       </c>
       <c r="N57" s="35" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O57" s="35" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="P57" s="32" t="s">
         <v>145</v>
@@ -7627,10 +7621,10 @@
       </c>
       <c r="T57" s="31"/>
       <c r="U57" s="33" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="V57" s="33" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
@@ -7638,7 +7632,7 @@
         <v>166</v>
       </c>
       <c r="B58" s="59" t="s">
-        <v>398</v>
+        <v>420</v>
       </c>
       <c r="C58" s="59" t="s">
         <v>395</v>
@@ -7674,10 +7668,10 @@
         <v>285</v>
       </c>
       <c r="N58" s="35" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="O58" s="35" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="P58" s="32" t="s">
         <v>145</v>
@@ -7691,10 +7685,10 @@
       </c>
       <c r="T58" s="31"/>
       <c r="U58" s="33" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="V58" s="62" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.2">
@@ -7702,7 +7696,7 @@
         <v>170</v>
       </c>
       <c r="B59" s="59" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C59" s="59" t="s">
         <v>395</v>
@@ -7751,13 +7745,13 @@
         <v>58</v>
       </c>
       <c r="S59" s="58" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="U59" s="59" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="V59" s="59" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.2">
@@ -7765,7 +7759,7 @@
         <v>201.1</v>
       </c>
       <c r="B60" s="59" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C60" s="59" t="s">
         <v>395</v>
@@ -7814,13 +7808,13 @@
         <v>58</v>
       </c>
       <c r="S60" s="58" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="U60" s="59" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="V60" s="59" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.2">
@@ -7828,7 +7822,7 @@
         <v>201.2</v>
       </c>
       <c r="B61" s="59" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C61" s="59" t="s">
         <v>395</v>
@@ -7877,13 +7871,13 @@
         <v>58</v>
       </c>
       <c r="S61" s="58" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="U61" s="59" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="V61" s="59" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.2">
@@ -7891,7 +7885,7 @@
         <v>202</v>
       </c>
       <c r="B62" s="59" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C62" s="59" t="s">
         <v>395</v>
@@ -7940,13 +7934,13 @@
         <v>58</v>
       </c>
       <c r="S62" s="58" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="U62" s="59" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="V62" s="59" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.2">
@@ -7954,7 +7948,7 @@
         <v>220</v>
       </c>
       <c r="B63" s="59" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C63" s="59" t="s">
         <v>395</v>
@@ -8003,13 +7997,13 @@
         <v>58</v>
       </c>
       <c r="S63" s="58" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="U63" s="59" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="V63" s="59" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.2">
@@ -8017,7 +8011,7 @@
         <v>221</v>
       </c>
       <c r="B64" s="59" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C64" s="59" t="s">
         <v>395</v>
@@ -8066,13 +8060,13 @@
         <v>58</v>
       </c>
       <c r="S64" s="58" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="U64" s="59" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="V64" s="59" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactoring EPV component (Dependoparvovirus)
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E38D917-E26D-8B42-911D-FB06BF71D4F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAEFFC6-C5A9-9D42-98D9-264FDF9F7DC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="3140" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11228" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11256" uniqueCount="523">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -1601,6 +1601,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>dependo.160-gymnobelideus</t>
+  </si>
+  <si>
+    <t>dependo.9-hyracoidea</t>
   </si>
 </sst>
 </file>
@@ -4231,16 +4237,16 @@
   <dimension ref="A1:AA64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="8" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" style="8" customWidth="1"/>
@@ -4418,11 +4424,11 @@
       <c r="W2" s="51">
         <v>27377618</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" s="5" t="s">
-        <v>165</v>
+      <c r="Y2" s="33" t="s">
+        <v>5</v>
       </c>
       <c r="Z2" s="33" t="s">
         <v>2</v>
@@ -4501,11 +4507,11 @@
       <c r="W3" s="51">
         <v>32913662</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="4" t="s">
-        <v>166</v>
+      <c r="Y3" s="33" t="s">
+        <v>6</v>
       </c>
       <c r="Z3" s="33" t="s">
         <v>2</v>
@@ -4582,11 +4588,11 @@
       <c r="W4" s="51">
         <v>32913662</v>
       </c>
-      <c r="X4" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>167</v>
+      <c r="X4" s="33" t="s">
+        <v>503</v>
+      </c>
+      <c r="Y4" s="33" t="s">
+        <v>503</v>
       </c>
       <c r="Z4" s="33" t="s">
         <v>2</v>
@@ -4665,11 +4671,11 @@
       <c r="W5" s="51">
         <v>32913662</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="X5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="4" t="s">
-        <v>168</v>
+      <c r="Y5" s="33" t="s">
+        <v>8</v>
       </c>
       <c r="Z5" s="33" t="s">
         <v>2</v>
@@ -4748,11 +4754,11 @@
       <c r="W6" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="X6" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="Y6" s="4" t="s">
-        <v>169</v>
+      <c r="Y6" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="Z6" s="33" t="s">
         <v>2</v>
@@ -4829,11 +4835,11 @@
       <c r="W7" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X7" s="4" t="s">
+      <c r="X7" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="Y7" s="4" t="s">
-        <v>175</v>
+      <c r="Y7" s="33" t="s">
+        <v>89</v>
       </c>
       <c r="Z7" s="33" t="s">
         <v>2</v>
@@ -4910,11 +4916,11 @@
       <c r="W8" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X8" s="4" t="s">
+      <c r="X8" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="Y8" s="4" t="s">
-        <v>186</v>
+      <c r="Y8" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="Z8" s="33" t="s">
         <v>2</v>
@@ -4989,10 +4995,18 @@
       <c r="W9" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="33"/>
-      <c r="AA9" s="33"/>
+      <c r="X9" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="Y9" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="Z9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="33" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
@@ -5062,11 +5076,11 @@
       <c r="W10" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X10" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>190</v>
+      <c r="X10" s="33" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y10" s="33" t="s">
+        <v>505</v>
       </c>
       <c r="Z10" s="33" t="s">
         <v>2</v>
@@ -5077,7 +5091,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>293</v>
+        <v>521</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>292</v>
@@ -5144,10 +5158,10 @@
         <v>520</v>
       </c>
       <c r="X11" s="33" t="s">
-        <v>293</v>
+        <v>521</v>
       </c>
       <c r="Y11" s="33" t="s">
-        <v>293</v>
+        <v>521</v>
       </c>
       <c r="Z11" s="33" t="s">
         <v>2</v>
@@ -5216,10 +5230,18 @@
       <c r="W12" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X12" s="56"/>
-      <c r="Y12" s="56"/>
-      <c r="Z12" s="54"/>
-      <c r="AA12" s="54"/>
+      <c r="X12" s="33" t="s">
+        <v>463</v>
+      </c>
+      <c r="Y12" s="33" t="s">
+        <v>463</v>
+      </c>
+      <c r="Z12" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="33" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
@@ -5291,8 +5313,12 @@
       <c r="W13" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
+      <c r="X13" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="Y13" s="33" t="s">
+        <v>411</v>
+      </c>
       <c r="Z13" s="33" t="s">
         <v>2</v>
       </c>
@@ -5370,8 +5396,12 @@
       <c r="W14" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
+      <c r="X14" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="Y14" s="33" t="s">
+        <v>413</v>
+      </c>
       <c r="Z14" s="33" t="s">
         <v>2</v>
       </c>
@@ -5447,11 +5477,11 @@
       <c r="W15" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="X15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="Y15" s="4" t="s">
-        <v>171</v>
+      <c r="Y15" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="Z15" s="33" t="s">
         <v>2</v>
@@ -5528,11 +5558,11 @@
       <c r="W16" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X16" s="4" t="s">
+      <c r="X16" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="Y16" s="4" t="s">
-        <v>172</v>
+      <c r="Y16" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="Z16" s="33" t="s">
         <v>2</v>
@@ -5543,7 +5573,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>114</v>
+        <v>522</v>
       </c>
       <c r="B17" s="33" t="s">
         <v>292</v>
@@ -5609,11 +5639,11 @@
       <c r="W17" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X17" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>244</v>
+      <c r="X17" s="33" t="s">
+        <v>522</v>
+      </c>
+      <c r="Y17" s="33" t="s">
+        <v>522</v>
       </c>
       <c r="Z17" s="33" t="s">
         <v>2</v>
@@ -5690,11 +5720,11 @@
       <c r="W18" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X18" s="4" t="s">
+      <c r="X18" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="Y18" s="4" t="s">
-        <v>174</v>
+      <c r="Y18" s="33" t="s">
+        <v>58</v>
       </c>
       <c r="Z18" s="33" t="s">
         <v>2</v>
@@ -5767,11 +5797,11 @@
       <c r="W19" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X19" s="4" t="s">
+      <c r="X19" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="Y19" s="4" t="s">
-        <v>176</v>
+      <c r="Y19" s="33" t="s">
+        <v>14</v>
       </c>
       <c r="Z19" s="33" t="s">
         <v>2</v>
@@ -5850,11 +5880,11 @@
       <c r="W20" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X20" s="4" t="s">
+      <c r="X20" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="Y20" s="4" t="s">
-        <v>178</v>
+      <c r="Y20" s="33" t="s">
+        <v>44</v>
       </c>
       <c r="Z20" s="33" t="s">
         <v>2</v>
@@ -5933,11 +5963,11 @@
       <c r="W21" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y21" s="4" t="s">
-        <v>179</v>
+      <c r="X21" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y21" s="33" t="s">
+        <v>115</v>
       </c>
       <c r="Z21" s="33" t="s">
         <v>2</v>
@@ -6014,11 +6044,11 @@
       <c r="W22" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X22" s="4" t="s">
+      <c r="X22" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="Y22" s="4" t="s">
-        <v>181</v>
+      <c r="Y22" s="33" t="s">
+        <v>201</v>
       </c>
       <c r="Z22" s="33" t="s">
         <v>2</v>
@@ -6097,11 +6127,11 @@
       <c r="W23" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X23" s="5" t="s">
+      <c r="X23" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="Y23" s="5" t="s">
-        <v>182</v>
+      <c r="Y23" s="33" t="s">
+        <v>117</v>
       </c>
       <c r="Z23" s="33" t="s">
         <v>2</v>
@@ -6178,11 +6208,11 @@
       <c r="W24" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X24" s="4" t="s">
+      <c r="X24" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="Y24" s="4" t="s">
-        <v>185</v>
+      <c r="Y24" s="33" t="s">
+        <v>86</v>
       </c>
       <c r="Z24" s="33" t="s">
         <v>2</v>
@@ -6259,11 +6289,11 @@
       <c r="W25" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X25" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="Y25" s="24" t="s">
-        <v>205</v>
+      <c r="X25" s="33" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y25" s="33" t="s">
+        <v>506</v>
       </c>
       <c r="Z25" s="33" t="s">
         <v>2</v>
@@ -6340,11 +6370,11 @@
       <c r="W26" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X26" s="4" t="s">
+      <c r="X26" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="Y26" s="4" t="s">
-        <v>253</v>
+      <c r="Y26" s="33" t="s">
+        <v>199</v>
       </c>
       <c r="Z26" s="33" t="s">
         <v>2</v>
@@ -6425,7 +6455,7 @@
         <v>198</v>
       </c>
       <c r="Y27" s="33" t="s">
-        <v>252</v>
+        <v>198</v>
       </c>
       <c r="Z27" s="33" t="s">
         <v>2</v>
@@ -6500,11 +6530,11 @@
       <c r="W28" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X28" s="4" t="s">
+      <c r="X28" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="Y28" s="4" t="s">
-        <v>189</v>
+      <c r="Y28" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="Z28" s="33" t="s">
         <v>2</v>
@@ -6581,11 +6611,11 @@
       <c r="W29" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X29" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="Y29" s="4" t="s">
-        <v>215</v>
+      <c r="X29" s="33" t="s">
+        <v>507</v>
+      </c>
+      <c r="Y29" s="33" t="s">
+        <v>507</v>
       </c>
       <c r="Z29" s="33" t="s">
         <v>2</v>
@@ -6625,10 +6655,18 @@
       <c r="J30" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="K30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="13"/>
@@ -6644,10 +6682,18 @@
       <c r="W30" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="33"/>
-      <c r="AA30" s="33"/>
+      <c r="X30" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y30" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z30" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA30" s="33" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
@@ -8809,7 +8855,30 @@
       <c r="H58" s="58"/>
       <c r="I58" s="58"/>
       <c r="J58" s="58"/>
-      <c r="R58" s="57"/>
+      <c r="K58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="L58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="M58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="N58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="O58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="P58" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q58" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="R58" s="57" t="s">
+        <v>158</v>
+      </c>
       <c r="S58" s="17" t="s">
         <v>498</v>
       </c>

</xml_diff>

<commit_message>
Refactor EPV component (dependo)
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30B932C-8E29-234F-A156-C7D328244448}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E322DA84-32BB-9E45-8E9D-8018FA110431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="3140" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11183" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11183" uniqueCount="529">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -1619,6 +1619,12 @@
   </si>
   <si>
     <t>dependo.30-chiroptera</t>
+  </si>
+  <si>
+    <t>dependo.48-mus</t>
+  </si>
+  <si>
+    <t>dependo.63-rodent</t>
   </si>
 </sst>
 </file>
@@ -4258,10 +4264,10 @@
   <dimension ref="A1:FH82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A56" sqref="A1:AA60"/>
+      <selection pane="bottomRight" activeCell="X41" sqref="A1:AA60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10738,11 +10744,11 @@
     </row>
     <row r="33" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>514</v>
+        <v>527</v>
       </c>
       <c r="B33" s="51"/>
       <c r="C33" s="51">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D33" s="59" t="s">
         <v>18</v>
@@ -12033,61 +12039,51 @@
     </row>
     <row r="39" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>463</v>
-      </c>
-      <c r="B39" s="51" t="s">
-        <v>121</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="B39" s="51"/>
       <c r="C39" s="51">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D39" s="59" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E39" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="F39" s="40" t="s">
-        <v>459</v>
-      </c>
-      <c r="G39" s="51">
-        <v>5</v>
-      </c>
-      <c r="H39" s="51">
-        <v>5</v>
-      </c>
-      <c r="I39" s="59" t="s">
-        <v>482</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="N39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="O39" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="P39" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q39" s="76" t="s">
-        <v>158</v>
+        <v>391</v>
+      </c>
+      <c r="F39" s="40"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q39" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="S39" s="17" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="T39" s="11" t="s">
         <v>62</v>
@@ -12099,10 +12095,10 @@
         <v>519</v>
       </c>
       <c r="W39" s="33" t="s">
-        <v>463</v>
+        <v>528</v>
       </c>
       <c r="X39" s="33" t="s">
-        <v>463</v>
+        <v>528</v>
       </c>
       <c r="Y39" s="33" t="s">
         <v>2</v>
@@ -12253,53 +12249,61 @@
     </row>
     <row r="40" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>515</v>
-      </c>
-      <c r="B40" s="51"/>
+        <v>463</v>
+      </c>
+      <c r="B40" s="51" t="s">
+        <v>121</v>
+      </c>
       <c r="C40" s="51">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D40" s="59" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E40" s="40" t="s">
-        <v>327</v>
-      </c>
-      <c r="F40" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q40" s="77" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" s="40" t="s">
+        <v>459</v>
+      </c>
+      <c r="G40" s="51">
+        <v>5</v>
+      </c>
+      <c r="H40" s="51">
+        <v>5</v>
+      </c>
+      <c r="I40" s="59" t="s">
         <v>482</v>
       </c>
+      <c r="J40" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q40" s="76" t="s">
+        <v>158</v>
+      </c>
       <c r="R40" s="17" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="S40" s="17" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="T40" s="11" t="s">
         <v>62</v>
@@ -12311,10 +12315,10 @@
         <v>519</v>
       </c>
       <c r="W40" s="33" t="s">
-        <v>515</v>
+        <v>463</v>
       </c>
       <c r="X40" s="33" t="s">
-        <v>515</v>
+        <v>463</v>
       </c>
       <c r="Y40" s="33" t="s">
         <v>2</v>
@@ -12465,73 +12469,68 @@
     </row>
     <row r="41" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>520</v>
-      </c>
-      <c r="B41" s="51" t="s">
+        <v>515</v>
+      </c>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51">
+        <v>92</v>
+      </c>
+      <c r="D41" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="40" t="s">
+        <v>327</v>
+      </c>
+      <c r="F41" s="38" t="s">
+        <v>483</v>
+      </c>
+      <c r="G41" s="59"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q41" s="77" t="s">
         <v>482</v>
       </c>
-      <c r="C41" s="51">
-        <v>160</v>
-      </c>
-      <c r="D41" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="38" t="s">
-        <v>459</v>
-      </c>
-      <c r="G41" s="51">
-        <v>1</v>
-      </c>
-      <c r="H41" s="51">
-        <v>1</v>
-      </c>
-      <c r="I41" s="59" t="s">
-        <v>482</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P41" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q41" s="17" t="s">
-        <v>482</v>
-      </c>
-      <c r="R41" s="18" t="s">
-        <v>489</v>
-      </c>
-      <c r="S41" s="18" t="s">
-        <v>489</v>
+      <c r="R41" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="S41" s="17" t="s">
+        <v>490</v>
       </c>
       <c r="T41" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="U41" s="11" t="s">
         <v>62</v>
       </c>
       <c r="V41" s="11" t="s">
         <v>519</v>
       </c>
       <c r="W41" s="33" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="X41" s="33" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="Y41" s="33" t="s">
         <v>2</v>
@@ -12682,66 +12681,73 @@
     </row>
     <row r="42" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>404</v>
-      </c>
-      <c r="B42" s="51"/>
+        <v>520</v>
+      </c>
+      <c r="B42" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C42" s="51">
-        <v>163</v>
-      </c>
-      <c r="D42" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="40" t="s">
-        <v>391</v>
-      </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P42" s="4" t="s">
+      <c r="E42" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="G42" s="51">
+        <v>1</v>
+      </c>
+      <c r="H42" s="51">
+        <v>1</v>
+      </c>
+      <c r="I42" s="59" t="s">
+        <v>482</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P42" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q42" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="R42" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="S42" s="17" t="s">
-        <v>497</v>
+        <v>482</v>
+      </c>
+      <c r="R42" s="18" t="s">
+        <v>489</v>
+      </c>
+      <c r="S42" s="18" t="s">
+        <v>489</v>
       </c>
       <c r="T42" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="U42" s="11" t="s">
         <v>62</v>
       </c>
       <c r="V42" s="11" t="s">
         <v>519</v>
       </c>
       <c r="W42" s="33" t="s">
-        <v>404</v>
+        <v>520</v>
       </c>
       <c r="X42" s="33" t="s">
-        <v>404</v>
+        <v>520</v>
       </c>
       <c r="Y42" s="33" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Refactor - dependo component
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E322DA84-32BB-9E45-8E9D-8018FA110431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A535EB-6644-B34C-BB2F-A2AF89FA3ABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10000" yWindow="3140" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11183" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11184" uniqueCount="530">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -1625,6 +1625,9 @@
   </si>
   <si>
     <t>dependo.63-rodent</t>
+  </si>
+  <si>
+    <t>dependo.180-rhinolophus</t>
   </si>
 </sst>
 </file>
@@ -4267,7 +4270,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X41" sqref="A1:AA60"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13336,7 +13339,7 @@
     </row>
     <row r="45" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
-        <v>417</v>
+        <v>529</v>
       </c>
       <c r="B45" s="51"/>
       <c r="C45" s="51">
@@ -13348,9 +13351,15 @@
       <c r="E45" s="40" t="s">
         <v>455</v>
       </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
+      <c r="F45" s="40" t="s">
+        <v>459</v>
+      </c>
+      <c r="G45" s="59">
+        <v>2</v>
+      </c>
+      <c r="H45" s="59">
+        <v>2</v>
+      </c>
       <c r="I45" s="59"/>
       <c r="J45" s="4" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Refactor dependo - new info on EVE expression
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-dependo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87048A0-6AC8-394C-A218-C62A83460DF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213D1F67-5C02-2742-9AEC-A98B7834AC02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="4040" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="3040" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11231" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11239" uniqueCount="533">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -4276,10 +4276,10 @@
   <dimension ref="A1:FH83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="L37" sqref="A1:AA62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5328,7 +5328,7 @@
       <c r="I8" s="51" t="s">
         <v>482</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K8" s="3" t="s">
@@ -5546,7 +5546,7 @@
       <c r="I9" s="51" t="s">
         <v>482</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -5982,7 +5982,7 @@
       <c r="I11" s="51" t="s">
         <v>482</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K11" s="3" t="s">
@@ -6414,7 +6414,7 @@
       <c r="I13" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K13" s="3" t="s">
@@ -6632,7 +6632,7 @@
       <c r="I14" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K14" s="3" t="s">
@@ -7070,7 +7070,7 @@
       <c r="I16" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K16" s="3" t="s">
@@ -7290,7 +7290,7 @@
       <c r="I17" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K17" s="3" t="s">
@@ -8606,7 +8606,7 @@
       <c r="I23" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K23" s="3" t="s">
@@ -9063,8 +9063,8 @@
       <c r="P25" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="Q25" s="76" t="s">
-        <v>158</v>
+      <c r="Q25" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="R25" s="18" t="s">
         <v>62</v>
@@ -9690,7 +9690,7 @@
       <c r="I28" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="J28" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K28" s="3" t="s">
@@ -9905,26 +9905,26 @@
       <c r="H29" s="59">
         <v>2</v>
       </c>
-      <c r="I29" s="33" t="s">
+      <c r="I29" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>62</v>
+      <c r="J29" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="P29" t="s">
         <v>121</v>
@@ -9947,19 +9947,19 @@
       <c r="V29" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="W29" t="s">
+      <c r="W29" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="X29" t="s">
+      <c r="X29" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="Y29" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z29" t="s">
+      <c r="Y29" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AA29" s="33" t="s">
         <v>3</v>
       </c>
       <c r="AB29" s="48"/>
@@ -11196,7 +11196,9 @@
       <c r="A35" s="33" t="s">
         <v>527</v>
       </c>
-      <c r="B35" s="51"/>
+      <c r="B35" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C35" s="51">
         <v>48</v>
       </c>
@@ -12491,7 +12493,9 @@
       <c r="A41" s="33" t="s">
         <v>528</v>
       </c>
-      <c r="B41" s="51"/>
+      <c r="B41" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C41" s="51">
         <v>63</v>
       </c>
@@ -12523,7 +12527,7 @@
       <c r="O41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P41" s="4" t="s">
+      <c r="P41" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q41" s="17" t="s">
@@ -12702,7 +12706,7 @@
         <v>463</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>121</v>
+        <v>482</v>
       </c>
       <c r="C42" s="51">
         <v>86</v>
@@ -12921,7 +12925,9 @@
       <c r="A43" s="33" t="s">
         <v>515</v>
       </c>
-      <c r="B43" s="51"/>
+      <c r="B43" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C43" s="51">
         <v>92</v>
       </c>
@@ -12934,8 +12940,12 @@
       <c r="F43" s="38" t="s">
         <v>483</v>
       </c>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
+      <c r="G43" s="59">
+        <v>1</v>
+      </c>
+      <c r="H43" s="59">
+        <v>1</v>
+      </c>
       <c r="I43" s="59"/>
       <c r="J43" s="4" t="s">
         <v>62</v>
@@ -12955,7 +12965,7 @@
       <c r="O43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P43" s="4" t="s">
+      <c r="P43" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q43" s="77" t="s">
@@ -13157,7 +13167,7 @@
       <c r="I44" s="59" t="s">
         <v>482</v>
       </c>
-      <c r="J44" s="3" t="s">
+      <c r="J44" s="21" t="s">
         <v>224</v>
       </c>
       <c r="K44" s="3" t="s">
@@ -13350,7 +13360,9 @@
       <c r="A45" s="33" t="s">
         <v>411</v>
       </c>
-      <c r="B45" s="51"/>
+      <c r="B45" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C45" s="51">
         <v>174</v>
       </c>
@@ -13390,7 +13402,7 @@
       <c r="O45" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="P45" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q45" s="76" t="s">
@@ -13569,7 +13581,7 @@
         <v>413</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>121</v>
+        <v>482</v>
       </c>
       <c r="C46" s="51">
         <v>177</v>
@@ -13788,7 +13800,9 @@
       <c r="A47" s="33" t="s">
         <v>529</v>
       </c>
-      <c r="B47" s="51"/>
+      <c r="B47" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C47" s="51">
         <v>180</v>
       </c>
@@ -13826,7 +13840,7 @@
       <c r="O47" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P47" s="4" t="s">
+      <c r="P47" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q47" s="76" t="s">
@@ -14036,7 +14050,7 @@
       <c r="O48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P48" s="4" t="s">
+      <c r="P48" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q48" s="76" t="s">
@@ -14214,7 +14228,9 @@
       <c r="A49" s="33" t="s">
         <v>517</v>
       </c>
-      <c r="B49" s="51"/>
+      <c r="B49" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C49" s="51">
         <v>191</v>
       </c>
@@ -14248,7 +14264,7 @@
       <c r="O49" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P49" s="4" t="s">
+      <c r="P49" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q49" s="76" t="s">
@@ -14424,7 +14440,9 @@
       <c r="A50" s="33" t="s">
         <v>518</v>
       </c>
-      <c r="B50" s="51"/>
+      <c r="B50" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C50" s="51">
         <v>192</v>
       </c>
@@ -14458,7 +14476,7 @@
       <c r="O50" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P50" s="4" t="s">
+      <c r="P50" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q50" s="76" t="s">
@@ -14671,7 +14689,7 @@
       <c r="O51" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P51" s="4" t="s">
+      <c r="P51" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q51" s="76" t="s">
@@ -14867,16 +14885,16 @@
       <c r="I52" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="J52" s="31" t="s">
+      <c r="J52" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="K52" s="31" t="s">
+      <c r="K52" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="L52" s="31" t="s">
+      <c r="L52" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="M52" s="31" t="s">
+      <c r="M52" s="3" t="s">
         <v>234</v>
       </c>
       <c r="N52" s="22" t="s">
@@ -14885,7 +14903,7 @@
       <c r="O52" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P52" s="4" t="s">
+      <c r="P52" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q52" s="76" t="s">
@@ -15098,7 +15116,7 @@
       <c r="O53" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P53" s="4" t="s">
+      <c r="P53" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q53" s="76" t="s">
@@ -15316,7 +15334,7 @@
       <c r="O54" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P54" s="4" t="s">
+      <c r="P54" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q54" s="76" t="s">
@@ -15494,7 +15512,9 @@
       <c r="A55" s="33" t="s">
         <v>471</v>
       </c>
-      <c r="B55" s="51"/>
+      <c r="B55" s="51" t="s">
+        <v>482</v>
+      </c>
       <c r="C55" s="51">
         <v>211</v>
       </c>
@@ -15528,7 +15548,7 @@
       <c r="O55" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P55" s="4" t="s">
+      <c r="P55" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q55" s="76" t="s">
@@ -15742,7 +15762,7 @@
       <c r="O56" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P56" s="4" t="s">
+      <c r="P56" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q56" s="76" t="s">
@@ -15962,7 +15982,7 @@
       <c r="O57" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P57" s="4" t="s">
+      <c r="P57" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q57" s="76" t="s">
@@ -16182,7 +16202,7 @@
       <c r="O58" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P58" s="4" t="s">
+      <c r="P58" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q58" s="76" t="s">
@@ -16398,7 +16418,7 @@
       <c r="O59" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P59" s="4" t="s">
+      <c r="P59" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q59" s="76" t="s">
@@ -16616,7 +16636,7 @@
       <c r="O60" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P60" s="4" t="s">
+      <c r="P60" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q60" s="76" t="s">
@@ -16836,7 +16856,7 @@
       <c r="O61" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P61" s="4" t="s">
+      <c r="P61" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q61" s="76" t="s">
@@ -17056,7 +17076,7 @@
       <c r="O62" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="P62" s="4" t="s">
+      <c r="P62" s="3" t="s">
         <v>121</v>
       </c>
       <c r="Q62" s="76" t="s">

</xml_diff>